<commit_message>
Correction to model descriptions; Adding main major references ; Adding responsible parties
</commit_message>
<xml_diff>
--- a/cmip6/citations/cmip6_ncc_citations.xlsx
+++ b/cmip6/citations/cmip6_ncc_citations.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
   <si>
     <t xml:space="preserve">ES-DOC CMIP6 Model Citations</t>
   </si>
@@ -72,6 +72,207 @@
   </si>
   <si>
     <t xml:space="preserve">http://journal.com/873487234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assur, A., 1958</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@inproceedings{ass58,
+    author = "A. Assur",
+    title = "{Composition of sea ice and its tensile strength}",
+    booktitle = "{Arctic Sea Ice; Conference held at Easton, Maryland, February 24-27, 1958}",
+    year = "1958",
+    pages = "10--138",
+    volume = "US 598",
+    publisher = "Publs. Natl. Res. Coun. Wash.",
+    address = "Washington, DC"}
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://hdl.handle.net/2027/uc1.31822020697603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Danabasoglu et al., 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://doi.org/10.1029/2019MS001916</t>
+  </si>
+  <si>
+    <t xml:space="preserve">article{https://doi.org/10.1029/2019MS001916,
+author = {Danabasoglu, G. and Lamarque, J.-F. and Bacmeister, J. and Bailey, D. A. and DuVivier, A. K.  and Edwards, J. and Emmons, L. K. and Fasullo, J. and Garcia, R. and Gettelman, A. and Hannay, C. and Holland, M. M. and Large, W. G. and Lauritzen, P. H. and Lawrence, D. M. and Lenaerts, J. T. M. and Lindsay, K. and Lipscomb, W. H. and Mills, M. J. and Neale, R. and Oleson, K. W. and Otto-Bliesner, B. and Phillips, A. S. and Sacks, W. and Tilmes, S. and van Kampenhout, L. and Vertenstein, M. and Bertini, A. and Dennis, J. and Deser, C. and Fischer, C. and Fox-Kemper, B. and Kay, J. E. and Kinnison, D. and Kushner, P. J. and Larson, V. E. and Long, M. C. and Mickelson, S. and Moore, J. K. and Nienhouse, E. and Polvani, L. and Rasch, P. J. and Strand, W. G.},
+title = {The Community Earth System Model Version 2 (CESM2)},
+journal = {Journal of Advances in Modeling Earth Systems},
+volume = {12},
+number = {2},
+pages = {e2019MS001916},
+keywords = {Community Earth System Model (CESM), global coupled Earth system modeling, preindustrial and historical simulations, coupled model development and evaluation},
+doi = {https://doi.org/10.1029/2019MS001916},
+url = {https://agupubs.onlinelibrary.wiley.com/doi/abs/10.1029/2019MS001916},
+eprint = {https://agupubs.onlinelibrary.wiley.com/doi/pdf/10.1029/2019MS001916},
+note = {e2019MS001916 2019MS001916},
+abstract = {Abstract An overview of the Community Earth System Model Version 2 (CESM2) is provided, including a discussion of the challenges encountered during its development and how they were addressed. In addition, an evaluation of a pair of CESM2 long preindustrial control and historical ensemble simulations is presented. These simulations were performed using the nominal 1° horizontal resolution configuration of the coupled model with both the “low-top” (40 km, with limited chemistry) and “high-top” (130 km, with comprehensive chemistry) versions of the atmospheric component. CESM2 contains many substantial science and infrastructure improvements and new capabilities since its previous major release, CESM1, resulting in improved historical simulations in comparison to CESM1 and available observations. These include major reductions in low-latitude precipitation and shortwave cloud forcing biases; better representation of the Madden-Julian Oscillation; better El Niño-Southern Oscillation-related teleconnections; and a global land carbon accumulation trend that agrees well with observationally based estimates. Most tropospheric and surface features of the low- and high-top simulations are very similar to each other, so these improvements are present in both configurations. CESM2 has an equilibrium climate sensitivity of 5.1–5.3 °C, larger than in CESM1, primarily due to a combination of relatively small changes to cloud microphysics and boundary layer parameters. In contrast, CESM2's transient climate response of 1.9–2.0 °C is comparable to that of CESM1. The model outputs from these and many other simulations are available to the research community, and they represent CESM2's contributions to the Coupled Model Intercomparison Project Phase 6.},
+year = {2020}
+}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://agupubs.onlinelibrary.wiley.com/doi/10.1029/2019MS001916</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dentener et al., 2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.5194/acp-6-4321-2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Article{acp-6-4321-2006,
+AUTHOR = {Dentener, F. and Kinne, S. and Bond, T. and Boucher, O. and Cofala, J. and Generoso, S. and Ginoux, P. and Gong, S. and Hoelzemann, J. J. and Ito, A. and Marelli, L. and Penner, J. E. and Putaud, J.-P. and Textor, C. and Schulz, M. and van der Werf, G. R. and Wilson, J.},
+TITLE = {Emissions of primary aerosol and precursor gases in the years 2000  and 1750 prescribed data-sets for AeroCom},
+JOURNAL = {Atmospheric Chemistry and Physics},
+VOLUME = {6},
+YEAR = {2006},
+NUMBER = {12},
+PAGES = {4321--4344},
+URL = {https://acp.copernicus.org/articles/6/4321/2006/},
+DOI = {10.5194/acp-6-4321-2006}
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://acp.copernicus.org/articles/6/4321/2006/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gliß et al., 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.5194/acp-21-87-2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Article{acp-21-87-2021,
+AUTHOR = {Gli{\ss}, J. and Mortier, A. and Schulz, M. and Andrews, E. and Balkanski, Y. and Bauer, S. E. and Benedictow, A. M. K. and Bian, H. and Checa-Garcia, R. and Chin, M. and Ginoux, P. and Griesfeller, J. J. and Heckel, A. and Kipling, Z. and Kirkev{\aa}g, A. and Kokkola, H. and Laj, P. and Le Sager, P. and Lund, M. T. and Lund Myhre, C. and Matsui, H. and Myhre, G. and Neubauer, D. and van Noije, T. and North, P. and Olivi\'e, D. J. L. and R\'emy, S. and Sogacheva, L. and Takemura, T. and Tsigaridis, K. and Tsyro, S. G.},
+TITLE = {AeroCom phase III multi-model evaluation of the aerosol life cycle and optical properties using ground- and space-based remote sensing as well as surface in situ observations},
+JOURNAL = {Atmospheric Chemistry and Physics},
+VOLUME = {21},
+YEAR = {2021},
+NUMBER = {1},
+PAGES = {87--128},
+URL = {https://acp.copernicus.org/articles/21/87/2021/},
+DOI = {10.5194/acp-21-87-2021}
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://acp.copernicus.org/articles/21/87/2021/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hunke_2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@techreport{Hunke2015,
+    author = "Elizabeth C. Hunke and William H. Lipscomb and Adrian K. Turner and Nicole Jeffery and Scott Elliott",
+    title = "{CICE: the Los Alamos Sea Ice Model Documentation and Software User’s Manual Version 5.1}",
+    institution = "Los Alamos National Laboratory",
+    year = "2015",
+    number = "LA-CC-06-012",
+    address = "Los Alamos, New Mexico, USA",
+    url = "https://github.com/CICE-Consortium/CICE-svn-trunk/releases/tag/cice-5.1.2"}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/CICE-Consortium/CICE-svn-trunk/releases/tag/cice-5.1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kirkevåg et al., 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.5194/gmd-11-3945-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Article{gmd-11-3945-2018,
+AUTHOR = {Kirkev{\aa}g, A. and Grini, A. and Olivi\'e, D. and Seland, {\O}. and Alterskj{\ae}r, K. and Hummel, M. and Karset, I. H. H. and Lewinschal, A. and Liu, X. and Makkonen, R. and Bethke, I. and Griesfeller, J. and Schulz, M. and Iversen, T.},
+TITLE = {A production-tagged aerosol module for Earth system models, OsloAero5.3 --
+extensions and updates for CAM5.3-Oslo},
+JOURNAL = {Geoscientific Model Development},
+VOLUME = {11},
+YEAR = {2018},
+NUMBER = {10},
+PAGES = {3945--3982},
+URL = {https://gmd.copernicus.org/articles/11/3945/2018/},
+DOI = {10.5194/gmd-11-3945-2018}
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://gmd.copernicus.org/articles/11/3945/2018/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lawrence_2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@article{lawrence_et_al_2019,
+author = {Lawrence, David M. and Fisher, Rosie A. and Koven, Charles D. and Oleson, Keith W. and Swenson, Sean C. and Bonan, Gordon and Collier, Nathan and Ghimire, Bardan and van Kampenhout, Leo and Kennedy, Daniel and Kluzek, Erik and Lawrence, Peter J. and Li, Fang and Li, Hongyi and Lombardozzi, Danica and Riley, William J. and Sacks, William J. and Shi, Mingjie and Vertenstein, Mariana and Wieder, William R. and Xu, Chonggang and Ali, Ashehad A. and Badger, Andrew M. and Bisht, Gautam and van den Broeke, Michiel and Brunke, Michael A. and Burns, Sean P. and Buzan, Jonathan and Clark, Martyn and Craig, Anthony and Dahlin, Kyla and Drewniak, Beth and Fisher, Joshua B. and Flanner, Mark and Fox, Andrew M. and Gentine, Pierre and Hoffman, Forrest and Keppel-Aleks, Gretchen and Knox, Ryan and Kumar, Sanjiv and Lenaerts, Jan and Leung, L. Ruby and Lipscomb, William H. and Lu, Yaqiong and Pandey, Ashutosh and Pelletier, Jon D. and Perket, Justin and Randerson, James T. and Ricciuto, Daniel M. and Sanderson, Benjamin M. and Slater, Andrew and Subin, Zachary M. and Tang, Jinyun and Thomas, R. Quinn and Val Martin, Maria and Zeng, Xubin},
+title = {The Community Land Model Version 5: Description of New Features, Benchmarking, and Impact of Forcing Uncertainty},
+journal = {Journal of Advances in Modeling Earth Systems},
+volume = {n/a},
+number = {n/a},
+pages = {},
+year = {2019},
+keywords = {global land model, Earth System Modeling, carbon and nitrogen cycling, hydrology, benchmarking},
+doi = {10.1029/2018MS001583},
+url = {https://agupubs.onlinelibrary.wiley.com/doi/abs/10.1029/2018MS001583},
+eprint = {https://agupubs.onlinelibrary.wiley.com/doi/pdf/10.1029/2018MS001583},
+}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://agupubs.onlinelibrary.wiley.com/doi/abs/10.1029/2018MS001583</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matthes et al., 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.5194/gmd-10-2247-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Article{gmd-10-2247-2017,
+AUTHOR = {Matthes, K. and Funke, B. and Andersson, M. E. and Barnard, L. and Beer, J. and Charbonneau, P. and Clilverd, M. A. and Dudok de Wit, T. and Haberreiter, M. and Hendry, A. and Jackman, C. H. and Kretzschmar, M. and Kruschke, T. and Kunze, M. and Langematz, U. and Marsh, D. R. and Maycock, A. C. and Misios, S. and Rodger, C. J. and Scaife, A. A. and Sepp\"al\"a, A. and Shangguan, M. and Sinnhuber, M. and Tourpali, K. and Usoskin, I. and van de Kamp, M. and Verronen, P. T. and Versick, S.},
+TITLE = {Solar forcing for CMIP6 (v3.2)},
+JOURNAL = {Geoscientific Model Development},
+VOLUME = {10},
+YEAR = {2017},
+NUMBER = {6},
+PAGES = {2247--2302},
+URL = {https://gmd.copernicus.org/articles/10/2247/2017/},
+DOI = {10.5194/gmd-10-2247-2017}
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://gmd.copernicus.org/articles/10/2247/2017/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seland et al., 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@article{doi:10.1111/j.1600-0870.2007.00313.x,
+author = {Alf Kirkevag and Trond Iversen and Øyvind Seland and Jens Boldingh Debernard and Trude Storelvmo and Jón Egill Kristjánsson},
+title = {Aerosol-cloud-climate interactions in the climate model CAM-Oslo},
+journal = {Tellus A: Dynamic Meteorology and Oceanography},
+volume = {60},
+number = {3},
+pages = {492-512},
+year  = {2008},
+publisher = {Taylor &amp; Francis},
+doi = {10.1111/j.1600-0870.2007.00313.x},
+URL = { 
+        https://www.tandfonline.com/doi/abs/10.1111/j.1600-0870.2007.00313.x
+},
+eprint = { 
+        https://www.tandfonline.com/doi/pdf/10.1111/j.1600-0870.2007.00313.x
+}
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.tandfonline.com/doi/abs/10.1111/j.1600-0870.2007.00313.x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seland et al., 2020</t>
   </si>
   <si>
     <t xml:space="preserve">https://doi.org/10.5194/gmd-13-6165-2020</t>
@@ -92,6 +293,50 @@
   <si>
     <t xml:space="preserve">https://gmd.copernicus.org/articles/13/6165/2020/</t>
   </si>
+  <si>
+    <t xml:space="preserve">Tjiputra et al., 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.5194/gmd-13-2393-2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Article{gmd-13-2393-2020,
+AUTHOR = {Tjiputra, J. F. and Schwinger, J. and Bentsen, M. and Mor\'ee, A. L. and Gao, S. and Bethke, I. and Heinze, C. and Goris, N. and Gupta, A. and He, Y.-C. and Olivi\'e, D. and Seland, {\O}. and Schulz, M.},
+TITLE = {Ocean biogeochemistry in the Norwegian Earth System Model version 2 (NorESM2)},
+JOURNAL = {Geoscientific Model Development},
+VOLUME = {13},
+YEAR = {2020},
+NUMBER = {5},
+PAGES = {2393--2431},
+URL = {https://gmd.copernicus.org/articles/13/2393/2020/},
+DOI = {10.5194/gmd-13-2393-2020}
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://gmd.copernicus.org/articles/13/2393/2020/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toniazzo et al. 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.5194/gmd-13-685-2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Article{gmd-13-685-2020,
+AUTHOR = {Toniazzo, T. and Bentsen, M. and Craig, C. and Eaton, B. E. and Edwards, J. and Goldhaber, S. and Jablonowski, C. and Lauritzen, P. H.},
+TITLE = {Enforcing conservation of axial angular momentum in the atmospheric general circulation model CAM6},
+JOURNAL = {Geoscientific Model Development},
+VOLUME = {13},
+YEAR = {2020},
+NUMBER = {2},
+PAGES = {685--705},
+URL = {https://gmd.copernicus.org/articles/13/685/2020/},
+DOI = {10.5194/gmd-13-685-2020}
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://gmd.copernicus.org/articles/13/685/2020/</t>
+  </si>
 </sst>
 </file>
 
@@ -101,7 +346,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Helvetica Neue"/>
@@ -197,6 +442,19 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Helvetica Neue"/>
+      <family val="0"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -295,7 +553,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -393,6 +651,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -951,10 +1225,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -996,106 +1270,188 @@
     </row>
     <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="22"/>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="23"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+    </row>
+    <row r="4" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="22"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+    </row>
+    <row r="5" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="B5" s="23"/>
+      <c r="C5" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D5" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="23"/>
-    </row>
-    <row r="4" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-    </row>
-    <row r="5" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-    </row>
-    <row r="6" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-    </row>
-    <row r="7" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-    </row>
-    <row r="8" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="18"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-    </row>
-    <row r="9" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-    </row>
-    <row r="10" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-    </row>
-    <row r="11" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="18"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-    </row>
-    <row r="12" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-    </row>
-    <row r="13" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
+      <c r="E5" s="23"/>
+    </row>
+    <row r="6" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="23"/>
+    </row>
+    <row r="8" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="23"/>
+    </row>
+    <row r="9" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="23"/>
+    </row>
+    <row r="10" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="23"/>
+    </row>
+    <row r="11" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="27"/>
+      <c r="C11" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="23"/>
+    </row>
+    <row r="12" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="23"/>
+    </row>
+    <row r="13" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="27"/>
+      <c r="C13" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="23"/>
     </row>
     <row r="14" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="18"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
+      <c r="A14" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>50</v>
+      </c>
       <c r="E14" s="19"/>
     </row>
     <row r="15" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="18"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
+      <c r="A15" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="E15" s="19"/>
     </row>
     <row r="16" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="18"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
+      <c r="A16" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>58</v>
+      </c>
       <c r="E16" s="19"/>
     </row>
     <row r="17" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1134,74 +1490,74 @@
       <c r="E21" s="19"/>
     </row>
     <row r="22" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="20"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
     </row>
     <row r="23" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="20"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
     </row>
     <row r="24" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="20"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
     </row>
     <row r="25" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="20"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
     </row>
     <row r="26" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="20"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
     </row>
     <row r="27" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="20"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
     </row>
     <row r="28" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="20"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
+      <c r="A28" s="18"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
     </row>
     <row r="29" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="20"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
     </row>
     <row r="30" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="20"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
+      <c r="A30" s="18"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
     </row>
     <row r="31" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="20"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
+      <c r="A31" s="18"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
     </row>
     <row r="32" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="20"/>
@@ -1350,10 +1706,95 @@
       <c r="D52" s="21"/>
       <c r="E52" s="21"/>
     </row>
+    <row r="53" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="20"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
+    </row>
+    <row r="54" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="20"/>
+      <c r="B54" s="21"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="21"/>
+    </row>
+    <row r="55" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="20"/>
+      <c r="B55" s="21"/>
+      <c r="C55" s="21"/>
+      <c r="D55" s="21"/>
+      <c r="E55" s="21"/>
+    </row>
+    <row r="56" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="20"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="21"/>
+    </row>
+    <row r="57" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="20"/>
+      <c r="B57" s="21"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
+    </row>
+    <row r="58" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="20"/>
+      <c r="B58" s="21"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+    </row>
+    <row r="59" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="20"/>
+      <c r="B59" s="21"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="21"/>
+    </row>
+    <row r="60" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="20"/>
+      <c r="B60" s="21"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="21"/>
+    </row>
+    <row r="61" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="20"/>
+      <c r="B61" s="21"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="21"/>
+    </row>
+    <row r="62" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="20"/>
+      <c r="B62" s="21"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="21"/>
+      <c r="E62" s="21"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="https://doi.org/10.5194/gmd-13-6165-2020"/>
-    <hyperlink ref="D3" r:id="rId2" display="https://gmd.copernicus.org/articles/13/6165/2020/"/>
+    <hyperlink ref="D5" r:id="rId1" display="https://hdl.handle.net/2027/uc1.31822020697603"/>
+    <hyperlink ref="B6" r:id="rId2" display=" https://doi.org/10.1029/2019MS001916"/>
+    <hyperlink ref="D6" r:id="rId3" display="https://agupubs.onlinelibrary.wiley.com/doi/10.1029/2019MS001916"/>
+    <hyperlink ref="B7" r:id="rId4" display="https://doi.org/10.5194/acp-6-4321-2006"/>
+    <hyperlink ref="D7" r:id="rId5" display="https://acp.copernicus.org/articles/6/4321/2006/"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://doi.org/10.5194/acp-21-87-2021"/>
+    <hyperlink ref="D9" r:id="rId7" display="https://github.com/CICE-Consortium/CICE-svn-trunk/releases/tag/cice-5.1.2"/>
+    <hyperlink ref="D11" r:id="rId8" display="https://agupubs.onlinelibrary.wiley.com/doi/abs/10.1029/2018MS001583"/>
+    <hyperlink ref="B12" r:id="rId9" display="https://doi.org/10.5194/gmd-10-2247-2017"/>
+    <hyperlink ref="D12" r:id="rId10" display="https://gmd.copernicus.org/articles/10/2247/2017/"/>
+    <hyperlink ref="D13" r:id="rId11" display="https://www.tandfonline.com/doi/abs/10.1111/j.1600-0870.2007.00313.x"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://doi.org/10.5194/gmd-13-6165-2020"/>
+    <hyperlink ref="D14" r:id="rId13" display="https://gmd.copernicus.org/articles/13/6165/2020/"/>
+    <hyperlink ref="B15" r:id="rId14" display="https://doi.org/10.5194/gmd-13-2393-2020"/>
+    <hyperlink ref="D15" r:id="rId15" display="https://gmd.copernicus.org/articles/13/2393/2020/"/>
+    <hyperlink ref="B16" r:id="rId16" display="https://doi.org/10.5194/gmd-13-685-2020"/>
+    <hyperlink ref="D16" r:id="rId17" display="https://gmd.copernicus.org/articles/13/685/2020/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.277777777777778"/>

</xml_diff>